<commit_message>
scale not optimizaed experiments
</commit_message>
<xml_diff>
--- a/Data/Excels/Drunkard/Resumes/Experiment 6.xlsx
+++ b/Data/Excels/Drunkard/Resumes/Experiment 6.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AL6"/>
+  <dimension ref="A1:DF6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -446,180 +446,540 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
+          <t>320_00000_1975-1983-InRays Improvement (%)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays Av. movement</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays Av. error</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays RMSE</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays parallax</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays nMatches</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-InRays nMPs</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints Av. movement</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints Av. error</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints RMSE</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints parallax</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints nMatches</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_1975-1983-TwoPoints nMPs</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
           <t>320_00000_1975-1983-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="V1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="W1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints Av. movement</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="X1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints Av. error</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="Y1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints RMSE</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="Z1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints t C1C2 norm (mm)</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="AA1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints parallax</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="AB1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints nMatches</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="AC1" s="1" t="inlineStr">
         <is>
           <t>320_00000_1975-1983-FarPoints nMPs</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays Improvement (%)</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays Av. movement</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays Av. error</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays RMSE</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays parallax</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays nMatches</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-InRays nMPs</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints Av. movement</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints Av. error</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints RMSE</t>
+        </is>
+      </c>
+      <c r="AR1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints parallax</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints nMatches</t>
+        </is>
+      </c>
+      <c r="AU1" s="1" t="inlineStr">
+        <is>
+          <t>320_00000_2500-2513-TwoPoints nMPs</t>
+        </is>
+      </c>
+      <c r="AV1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="AW1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="AX1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints Av. movement</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="AY1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints Av. error</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="AZ1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints RMSE</t>
         </is>
       </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="BA1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints t C1C2 norm (mm)</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="BB1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints parallax</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="BC1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints nMatches</t>
         </is>
       </c>
-      <c r="T1" s="1" t="inlineStr">
+      <c r="BD1" s="1" t="inlineStr">
         <is>
           <t>320_00000_2500-2513-FarPoints nMPs</t>
         </is>
       </c>
-      <c r="U1" s="1" t="inlineStr">
+      <c r="BE1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays Improvement (%)</t>
+        </is>
+      </c>
+      <c r="BF1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="BG1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays Av. movement</t>
+        </is>
+      </c>
+      <c r="BH1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays Av. error</t>
+        </is>
+      </c>
+      <c r="BI1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays RMSE</t>
+        </is>
+      </c>
+      <c r="BJ1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="BK1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays parallax</t>
+        </is>
+      </c>
+      <c r="BL1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays nMatches</t>
+        </is>
+      </c>
+      <c r="BM1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-InRays nMPs</t>
+        </is>
+      </c>
+      <c r="BN1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="BO1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="BP1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints Av. movement</t>
+        </is>
+      </c>
+      <c r="BQ1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints Av. error</t>
+        </is>
+      </c>
+      <c r="BR1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints RMSE</t>
+        </is>
+      </c>
+      <c r="BS1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="BT1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints parallax</t>
+        </is>
+      </c>
+      <c r="BU1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints nMatches</t>
+        </is>
+      </c>
+      <c r="BV1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00000_1229-1236-TwoPoints nMPs</t>
+        </is>
+      </c>
+      <c r="BW1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="V1" s="1" t="inlineStr">
+      <c r="BX1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="W1" s="1" t="inlineStr">
+      <c r="BY1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints Av. movement</t>
         </is>
       </c>
-      <c r="X1" s="1" t="inlineStr">
+      <c r="BZ1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints Av. error</t>
         </is>
       </c>
-      <c r="Y1" s="1" t="inlineStr">
+      <c r="CA1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints RMSE</t>
         </is>
       </c>
-      <c r="Z1" s="1" t="inlineStr">
+      <c r="CB1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints t C1C2 norm (mm)</t>
         </is>
       </c>
-      <c r="AA1" s="1" t="inlineStr">
+      <c r="CC1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints parallax</t>
         </is>
       </c>
-      <c r="AB1" s="1" t="inlineStr">
+      <c r="CD1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints nMatches</t>
         </is>
       </c>
-      <c r="AC1" s="1" t="inlineStr">
+      <c r="CE1" s="1" t="inlineStr">
         <is>
           <t>1024_00000_1229-1236-FarPoints nMPs</t>
         </is>
       </c>
-      <c r="AD1" s="1" t="inlineStr">
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays Improvement (%)</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays Av. movement</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays Av. error</t>
+        </is>
+      </c>
+      <c r="CJ1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays RMSE</t>
+        </is>
+      </c>
+      <c r="CK1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays parallax</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays nMatches</t>
+        </is>
+      </c>
+      <c r="CN1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-InRays nMPs</t>
+        </is>
+      </c>
+      <c r="CO1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints Improvement (%)</t>
+        </is>
+      </c>
+      <c r="CP1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints Final Vs Mov (%)</t>
+        </is>
+      </c>
+      <c r="CQ1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints Av. movement</t>
+        </is>
+      </c>
+      <c r="CR1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints Av. error</t>
+        </is>
+      </c>
+      <c r="CS1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints RMSE</t>
+        </is>
+      </c>
+      <c r="CT1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints t C1C2 norm (mm)</t>
+        </is>
+      </c>
+      <c r="CU1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints parallax</t>
+        </is>
+      </c>
+      <c r="CV1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints nMatches</t>
+        </is>
+      </c>
+      <c r="CW1" s="1" t="inlineStr">
+        <is>
+          <t>1024_00001_110-120-TwoPoints nMPs</t>
+        </is>
+      </c>
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints Improvement (%)</t>
         </is>
       </c>
-      <c r="AE1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints Final Vs Mov (%)</t>
         </is>
       </c>
-      <c r="AF1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints Av. movement</t>
         </is>
       </c>
-      <c r="AG1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints Av. error</t>
         </is>
       </c>
-      <c r="AH1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints RMSE</t>
         </is>
       </c>
-      <c r="AI1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints t C1C2 norm (mm)</t>
         </is>
       </c>
-      <c r="AJ1" s="1" t="inlineStr">
+      <c r="DD1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints parallax</t>
         </is>
       </c>
-      <c r="AK1" s="1" t="inlineStr">
+      <c r="DE1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints nMatches</t>
         </is>
       </c>
-      <c r="AL1" s="1" t="inlineStr">
+      <c r="DF1" s="1" t="inlineStr">
         <is>
           <t>1024_00001_110-120-FarPoints nMPs</t>
         </is>
@@ -637,19 +997,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>-459.78</v>
+        <v>-466.55</v>
       </c>
       <c r="D2" t="n">
-        <v>18687.29</v>
+        <v>18603.56</v>
       </c>
       <c r="E2" t="n">
-        <v>7.75</v>
+        <v>7.95</v>
       </c>
       <c r="F2" t="n">
-        <v>1447.65</v>
+        <v>1478.57</v>
       </c>
       <c r="G2" t="n">
-        <v>1457.97</v>
+        <v>1488.93</v>
       </c>
       <c r="H2" t="n">
         <v>31.47</v>
@@ -661,87 +1021,303 @@
         <v>216</v>
       </c>
       <c r="K2" t="n">
+        <v>412</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-59.21</v>
+      </c>
+      <c r="M2" t="n">
+        <v>5314.68</v>
+      </c>
+      <c r="N2" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="O2" t="n">
+        <v>411.71</v>
+      </c>
+      <c r="P2" t="n">
+        <v>440.55</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>31.47</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="S2" t="n">
+        <v>216</v>
+      </c>
+      <c r="T2" t="n">
         <v>410</v>
       </c>
-      <c r="L2" t="n">
+      <c r="U2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="V2" t="n">
+        <v>3335.78</v>
+      </c>
+      <c r="W2" t="n">
+        <v>7.75</v>
+      </c>
+      <c r="X2" t="n">
+        <v>258.41</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>356.83</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>31.47</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>216</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>410</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>27.23</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>789.9400000000001</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>31.83</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>251.43</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>298.22</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>110.08</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>164</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>286</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>19.55</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>1238.57</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>17.98</v>
+      </c>
+      <c r="AP2" t="n">
+        <v>222.75</v>
+      </c>
+      <c r="AQ2" t="n">
+        <v>339.27</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>110.08</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>1.69</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>164</v>
+      </c>
+      <c r="AU2" t="n">
+        <v>272</v>
+      </c>
+      <c r="AV2" t="n">
         <v>19.88</v>
       </c>
-      <c r="M2" t="n">
+      <c r="AW2" t="n">
         <v>1233.49</v>
       </c>
-      <c r="N2" t="n">
+      <c r="AX2" t="n">
         <v>17.98</v>
       </c>
-      <c r="O2" t="n">
+      <c r="AY2" t="n">
         <v>221.84</v>
       </c>
-      <c r="P2" t="n">
+      <c r="AZ2" t="n">
         <v>341.52</v>
       </c>
-      <c r="Q2" t="n">
+      <c r="BA2" t="n">
         <v>110.08</v>
       </c>
-      <c r="R2" t="n">
+      <c r="BB2" t="n">
         <v>1.69</v>
       </c>
-      <c r="S2" t="n">
+      <c r="BC2" t="n">
         <v>164</v>
       </c>
-      <c r="T2" t="n">
+      <c r="BD2" t="n">
         <v>272</v>
       </c>
-      <c r="U2" t="n">
+      <c r="BE2" t="n">
+        <v>3.43</v>
+      </c>
+      <c r="BF2" t="n">
+        <v>1042.9</v>
+      </c>
+      <c r="BG2" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>58.04</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>176.49</v>
+      </c>
+      <c r="BJ2" t="n">
+        <v>131.58</v>
+      </c>
+      <c r="BK2" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL2" t="n">
+        <v>109</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>218</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>96.27</v>
+      </c>
+      <c r="BO2" t="n">
+        <v>55.15</v>
+      </c>
+      <c r="BP2" t="n">
+        <v>2.58</v>
+      </c>
+      <c r="BQ2" t="n">
+        <v>1.42</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>131.58</v>
+      </c>
+      <c r="BT2" t="n">
+        <v>1.96</v>
+      </c>
+      <c r="BU2" t="n">
+        <v>109</v>
+      </c>
+      <c r="BV2" t="n">
+        <v>214</v>
+      </c>
+      <c r="BW2" t="n">
         <v>95.97</v>
       </c>
-      <c r="V2" t="n">
+      <c r="BX2" t="n">
         <v>59.35</v>
       </c>
-      <c r="W2" t="n">
+      <c r="BY2" t="n">
         <v>2.58</v>
       </c>
-      <c r="X2" t="n">
+      <c r="BZ2" t="n">
         <v>1.53</v>
       </c>
-      <c r="Y2" t="n">
+      <c r="CA2" t="n">
         <v>1.71</v>
       </c>
-      <c r="Z2" t="n">
+      <c r="CB2" t="n">
         <v>131.58</v>
       </c>
-      <c r="AA2" t="n">
+      <c r="CC2" t="n">
         <v>1.96</v>
       </c>
-      <c r="AB2" t="n">
+      <c r="CD2" t="n">
         <v>109</v>
       </c>
-      <c r="AC2" t="n">
+      <c r="CE2" t="n">
         <v>214</v>
       </c>
-      <c r="AD2" t="n">
+      <c r="CF2" t="n">
+        <v>10.35</v>
+      </c>
+      <c r="CG2" t="n">
+        <v>1243.46</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>15.53</v>
+      </c>
+      <c r="CI2" t="n">
+        <v>193.06</v>
+      </c>
+      <c r="CJ2" t="n">
+        <v>360.46</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>74.84</v>
+      </c>
+      <c r="CL2" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>93</v>
+      </c>
+      <c r="CN2" t="n">
+        <v>186</v>
+      </c>
+      <c r="CO2" t="n">
+        <v>79.44</v>
+      </c>
+      <c r="CP2" t="n">
+        <v>279.73</v>
+      </c>
+      <c r="CQ2" t="n">
+        <v>14.68</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>41.08</v>
+      </c>
+      <c r="CS2" t="n">
+        <v>42.72</v>
+      </c>
+      <c r="CT2" t="n">
+        <v>74.84</v>
+      </c>
+      <c r="CU2" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>93</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>184</v>
+      </c>
+      <c r="CX2" t="n">
         <v>81.94</v>
       </c>
-      <c r="AE2" t="n">
+      <c r="CY2" t="n">
         <v>245.75</v>
       </c>
-      <c r="AF2" t="n">
+      <c r="CZ2" t="n">
         <v>14.68</v>
       </c>
-      <c r="AG2" t="n">
+      <c r="DA2" t="n">
         <v>36.09</v>
       </c>
-      <c r="AH2" t="n">
+      <c r="DB2" t="n">
         <v>37.7</v>
       </c>
-      <c r="AI2" t="n">
+      <c r="DC2" t="n">
         <v>74.84</v>
       </c>
-      <c r="AJ2" t="n">
+      <c r="DD2" t="n">
         <v>0.6899999999999999</v>
       </c>
-      <c r="AK2" t="n">
+      <c r="DE2" t="n">
         <v>93</v>
       </c>
-      <c r="AL2" t="n">
+      <c r="DF2" t="n">
         <v>184</v>
       </c>
     </row>
@@ -757,19 +1333,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>-412.64</v>
+        <v>-466.55</v>
       </c>
       <c r="D3" t="n">
-        <v>16836.15</v>
+        <v>18603.56</v>
       </c>
       <c r="E3" t="n">
         <v>7.95</v>
       </c>
       <c r="F3" t="n">
-        <v>1338.1</v>
+        <v>1478.57</v>
       </c>
       <c r="G3" t="n">
-        <v>1347.49</v>
+        <v>1488.93</v>
       </c>
       <c r="H3" t="n">
         <v>31.47</v>
@@ -784,84 +1360,300 @@
         <v>412</v>
       </c>
       <c r="L3" t="n">
+        <v>20.43</v>
+      </c>
+      <c r="M3" t="n">
+        <v>2613.11</v>
+      </c>
+      <c r="N3" t="n">
+        <v>7.95</v>
+      </c>
+      <c r="O3" t="n">
+        <v>207.68</v>
+      </c>
+      <c r="P3" t="n">
+        <v>290.12</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>31.47</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="S3" t="n">
+        <v>216</v>
+      </c>
+      <c r="T3" t="n">
+        <v>412</v>
+      </c>
+      <c r="U3" t="n">
+        <v>-388.82</v>
+      </c>
+      <c r="V3" t="n">
+        <v>16053.92</v>
+      </c>
+      <c r="W3" t="n">
+        <v>7.95</v>
+      </c>
+      <c r="X3" t="n">
+        <v>1275.93</v>
+      </c>
+      <c r="Y3" t="n">
+        <v>1285.75</v>
+      </c>
+      <c r="Z3" t="n">
+        <v>31.47</v>
+      </c>
+      <c r="AA3" t="n">
+        <v>0.77</v>
+      </c>
+      <c r="AB3" t="n">
+        <v>216</v>
+      </c>
+      <c r="AC3" t="n">
+        <v>412</v>
+      </c>
+      <c r="AD3" t="n">
+        <v>27.23</v>
+      </c>
+      <c r="AE3" t="n">
+        <v>789.9400000000001</v>
+      </c>
+      <c r="AF3" t="n">
+        <v>31.83</v>
+      </c>
+      <c r="AG3" t="n">
+        <v>251.43</v>
+      </c>
+      <c r="AH3" t="n">
+        <v>298.22</v>
+      </c>
+      <c r="AI3" t="n">
+        <v>110.08</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>164</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>286</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>-487.45</v>
+      </c>
+      <c r="AN3" t="n">
+        <v>6381.5</v>
+      </c>
+      <c r="AO3" t="n">
+        <v>31.83</v>
+      </c>
+      <c r="AP3" t="n">
+        <v>2031.13</v>
+      </c>
+      <c r="AQ3" t="n">
+        <v>2055.66</v>
+      </c>
+      <c r="AR3" t="n">
+        <v>110.08</v>
+      </c>
+      <c r="AS3" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="AT3" t="n">
+        <v>164</v>
+      </c>
+      <c r="AU3" t="n">
+        <v>286</v>
+      </c>
+      <c r="AV3" t="n">
         <v>-459.67</v>
       </c>
-      <c r="M3" t="n">
+      <c r="AW3" t="n">
         <v>6075.77</v>
       </c>
-      <c r="N3" t="n">
+      <c r="AX3" t="n">
         <v>31.83</v>
       </c>
-      <c r="O3" t="n">
+      <c r="AY3" t="n">
         <v>1933.82</v>
       </c>
-      <c r="P3" t="n">
+      <c r="AZ3" t="n">
         <v>1957.21</v>
       </c>
-      <c r="Q3" t="n">
+      <c r="BA3" t="n">
         <v>110.08</v>
       </c>
-      <c r="R3" t="n">
+      <c r="BB3" t="n">
         <v>1.71</v>
       </c>
-      <c r="S3" t="n">
+      <c r="BC3" t="n">
         <v>164</v>
       </c>
-      <c r="T3" t="n">
+      <c r="BD3" t="n">
         <v>286</v>
       </c>
-      <c r="U3" t="n">
+      <c r="BE3" t="n">
+        <v>1.19</v>
+      </c>
+      <c r="BF3" t="n">
+        <v>1065.95</v>
+      </c>
+      <c r="BG3" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="BH3" t="n">
+        <v>59.39</v>
+      </c>
+      <c r="BI3" t="n">
+        <v>179.33</v>
+      </c>
+      <c r="BJ3" t="n">
+        <v>131.58</v>
+      </c>
+      <c r="BK3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BL3" t="n">
+        <v>109</v>
+      </c>
+      <c r="BM3" t="n">
+        <v>218</v>
+      </c>
+      <c r="BN3" t="n">
+        <v>-0.16</v>
+      </c>
+      <c r="BO3" t="n">
+        <v>1080.84</v>
+      </c>
+      <c r="BP3" t="n">
+        <v>5.57</v>
+      </c>
+      <c r="BQ3" t="n">
+        <v>60.22</v>
+      </c>
+      <c r="BR3" t="n">
+        <v>181.1</v>
+      </c>
+      <c r="BS3" t="n">
+        <v>131.58</v>
+      </c>
+      <c r="BT3" t="n">
+        <v>2</v>
+      </c>
+      <c r="BU3" t="n">
+        <v>109</v>
+      </c>
+      <c r="BV3" t="n">
+        <v>218</v>
+      </c>
+      <c r="BW3" t="n">
         <v>32.27</v>
       </c>
-      <c r="V3" t="n">
+      <c r="BX3" t="n">
         <v>738.49</v>
       </c>
-      <c r="W3" t="n">
+      <c r="BY3" t="n">
         <v>5.57</v>
       </c>
-      <c r="X3" t="n">
+      <c r="BZ3" t="n">
         <v>41.14</v>
       </c>
-      <c r="Y3" t="n">
+      <c r="CA3" t="n">
         <v>128.34</v>
       </c>
-      <c r="Z3" t="n">
+      <c r="CB3" t="n">
         <v>131.58</v>
       </c>
-      <c r="AA3" t="n">
+      <c r="CC3" t="n">
         <v>2</v>
       </c>
-      <c r="AB3" t="n">
+      <c r="CD3" t="n">
         <v>110</v>
       </c>
-      <c r="AC3" t="n">
+      <c r="CE3" t="n">
         <v>220</v>
       </c>
-      <c r="AD3" t="n">
+      <c r="CF3" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="CG3" t="n">
+        <v>1300.99</v>
+      </c>
+      <c r="CH3" t="n">
+        <v>15.53</v>
+      </c>
+      <c r="CI3" t="n">
+        <v>201.99</v>
+      </c>
+      <c r="CJ3" t="n">
+        <v>376.4</v>
+      </c>
+      <c r="CK3" t="n">
+        <v>74.84</v>
+      </c>
+      <c r="CL3" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="CM3" t="n">
+        <v>93</v>
+      </c>
+      <c r="CN3" t="n">
+        <v>186</v>
+      </c>
+      <c r="CO3" t="n">
+        <v>84.86</v>
+      </c>
+      <c r="CP3" t="n">
+        <v>209.97</v>
+      </c>
+      <c r="CQ3" t="n">
+        <v>15.53</v>
+      </c>
+      <c r="CR3" t="n">
+        <v>32.6</v>
+      </c>
+      <c r="CS3" t="n">
+        <v>33.83</v>
+      </c>
+      <c r="CT3" t="n">
+        <v>74.84</v>
+      </c>
+      <c r="CU3" t="n">
+        <v>0.74</v>
+      </c>
+      <c r="CV3" t="n">
+        <v>93</v>
+      </c>
+      <c r="CW3" t="n">
+        <v>186</v>
+      </c>
+      <c r="CX3" t="n">
         <v>5.01</v>
       </c>
-      <c r="AE3" t="n">
+      <c r="CY3" t="n">
         <v>1347.06</v>
       </c>
-      <c r="AF3" t="n">
+      <c r="CZ3" t="n">
         <v>15.27</v>
       </c>
-      <c r="AG3" t="n">
+      <c r="DA3" t="n">
         <v>205.75</v>
       </c>
-      <c r="AH3" t="n">
+      <c r="DB3" t="n">
         <v>379.12</v>
       </c>
-      <c r="AI3" t="n">
+      <c r="DC3" t="n">
         <v>74.84</v>
       </c>
-      <c r="AJ3" t="n">
+      <c r="DD3" t="n">
         <v>0.74</v>
       </c>
-      <c r="AK3" t="n">
+      <c r="DE3" t="n">
         <v>95</v>
       </c>
-      <c r="AL3" t="n">
+      <c r="DF3" t="n">
         <v>190</v>
       </c>
     </row>
@@ -877,19 +1669,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>76.53</v>
+        <v>55.37</v>
       </c>
       <c r="D4" t="n">
-        <v>806.22</v>
+        <v>1532.82</v>
       </c>
       <c r="E4" t="n">
         <v>29.35</v>
       </c>
       <c r="F4" t="n">
-        <v>236.61</v>
+        <v>449.85</v>
       </c>
       <c r="G4" t="n">
-        <v>326.64</v>
+        <v>502.84</v>
       </c>
       <c r="H4" t="n">
         <v>46.97</v>
@@ -904,84 +1696,300 @@
         <v>330</v>
       </c>
       <c r="L4" t="n">
+        <v>21.65</v>
+      </c>
+      <c r="M4" t="n">
+        <v>2691.38</v>
+      </c>
+      <c r="N4" t="n">
+        <v>29.35</v>
+      </c>
+      <c r="O4" t="n">
+        <v>789.86</v>
+      </c>
+      <c r="P4" t="n">
+        <v>815.52</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>46.97</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="S4" t="n">
+        <v>185</v>
+      </c>
+      <c r="T4" t="n">
+        <v>330</v>
+      </c>
+      <c r="U4" t="n">
+        <v>76.53</v>
+      </c>
+      <c r="V4" t="n">
+        <v>806.22</v>
+      </c>
+      <c r="W4" t="n">
+        <v>29.35</v>
+      </c>
+      <c r="X4" t="n">
+        <v>236.61</v>
+      </c>
+      <c r="Y4" t="n">
+        <v>326.64</v>
+      </c>
+      <c r="Z4" t="n">
+        <v>46.97</v>
+      </c>
+      <c r="AA4" t="n">
+        <v>0.6899999999999999</v>
+      </c>
+      <c r="AB4" t="n">
+        <v>185</v>
+      </c>
+      <c r="AC4" t="n">
+        <v>330</v>
+      </c>
+      <c r="AD4" t="n">
+        <v>-330.64</v>
+      </c>
+      <c r="AE4" t="n">
+        <v>4565.99</v>
+      </c>
+      <c r="AF4" t="n">
+        <v>38.4</v>
+      </c>
+      <c r="AG4" t="n">
+        <v>1753.25</v>
+      </c>
+      <c r="AH4" t="n">
+        <v>1782.37</v>
+      </c>
+      <c r="AI4" t="n">
+        <v>139.43</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>193</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>342</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>66.77</v>
+      </c>
+      <c r="AN4" t="n">
+        <v>350.56</v>
+      </c>
+      <c r="AO4" t="n">
+        <v>38.38</v>
+      </c>
+      <c r="AP4" t="n">
+        <v>134.54</v>
+      </c>
+      <c r="AQ4" t="n">
+        <v>196.21</v>
+      </c>
+      <c r="AR4" t="n">
+        <v>139.43</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>1.62</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>193</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>340</v>
+      </c>
+      <c r="AV4" t="n">
         <v>-130.85</v>
       </c>
-      <c r="M4" t="n">
+      <c r="AW4" t="n">
         <v>2435.4</v>
       </c>
-      <c r="N4" t="n">
+      <c r="AX4" t="n">
         <v>38.38</v>
       </c>
-      <c r="O4" t="n">
+      <c r="AY4" t="n">
         <v>934.65</v>
       </c>
-      <c r="P4" t="n">
+      <c r="AZ4" t="n">
         <v>951.59</v>
       </c>
-      <c r="Q4" t="n">
+      <c r="BA4" t="n">
         <v>139.43</v>
       </c>
-      <c r="R4" t="n">
+      <c r="BB4" t="n">
         <v>1.62</v>
       </c>
-      <c r="S4" t="n">
+      <c r="BC4" t="n">
         <v>193</v>
       </c>
-      <c r="T4" t="n">
+      <c r="BD4" t="n">
         <v>340</v>
       </c>
-      <c r="U4" t="n">
+      <c r="BE4" t="n">
+        <v>78.8</v>
+      </c>
+      <c r="BF4" t="n">
+        <v>89.45</v>
+      </c>
+      <c r="BG4" t="n">
+        <v>34.42</v>
+      </c>
+      <c r="BH4" t="n">
+        <v>30.79</v>
+      </c>
+      <c r="BI4" t="n">
+        <v>32.32</v>
+      </c>
+      <c r="BJ4" t="n">
+        <v>131.67</v>
+      </c>
+      <c r="BK4" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="BL4" t="n">
+        <v>86</v>
+      </c>
+      <c r="BM4" t="n">
+        <v>152</v>
+      </c>
+      <c r="BN4" t="n">
+        <v>24.05</v>
+      </c>
+      <c r="BO4" t="n">
+        <v>323.73</v>
+      </c>
+      <c r="BP4" t="n">
+        <v>34.42</v>
+      </c>
+      <c r="BQ4" t="n">
+        <v>111.42</v>
+      </c>
+      <c r="BR4" t="n">
+        <v>236.47</v>
+      </c>
+      <c r="BS4" t="n">
+        <v>131.67</v>
+      </c>
+      <c r="BT4" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="BU4" t="n">
+        <v>86</v>
+      </c>
+      <c r="BV4" t="n">
+        <v>152</v>
+      </c>
+      <c r="BW4" t="n">
         <v>79.01000000000001</v>
       </c>
-      <c r="V4" t="n">
+      <c r="BX4" t="n">
         <v>89.42</v>
       </c>
-      <c r="W4" t="n">
+      <c r="BY4" t="n">
         <v>34.42</v>
       </c>
-      <c r="X4" t="n">
+      <c r="BZ4" t="n">
         <v>30.77</v>
       </c>
-      <c r="Y4" t="n">
+      <c r="CA4" t="n">
         <v>31.68</v>
       </c>
-      <c r="Z4" t="n">
+      <c r="CB4" t="n">
         <v>131.67</v>
       </c>
-      <c r="AA4" t="n">
+      <c r="CC4" t="n">
         <v>2.05</v>
       </c>
-      <c r="AB4" t="n">
+      <c r="CD4" t="n">
         <v>86</v>
       </c>
-      <c r="AC4" t="n">
+      <c r="CE4" t="n">
         <v>152</v>
       </c>
-      <c r="AD4" t="n">
+      <c r="CF4" t="n">
         <v>47.68</v>
       </c>
-      <c r="AE4" t="n">
+      <c r="CG4" t="n">
+        <v>878.4299999999999</v>
+      </c>
+      <c r="CH4" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="CI4" t="n">
+        <v>217.86</v>
+      </c>
+      <c r="CJ4" t="n">
+        <v>224.45</v>
+      </c>
+      <c r="CK4" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="CL4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="CM4" t="n">
+        <v>99</v>
+      </c>
+      <c r="CN4" t="n">
+        <v>198</v>
+      </c>
+      <c r="CO4" t="n">
+        <v>47.7</v>
+      </c>
+      <c r="CP4" t="n">
+        <v>878.3200000000001</v>
+      </c>
+      <c r="CQ4" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="CR4" t="n">
+        <v>217.84</v>
+      </c>
+      <c r="CS4" t="n">
+        <v>224.48</v>
+      </c>
+      <c r="CT4" t="n">
+        <v>71.09999999999999</v>
+      </c>
+      <c r="CU4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="CV4" t="n">
+        <v>99</v>
+      </c>
+      <c r="CW4" t="n">
+        <v>198</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>47.68</v>
+      </c>
+      <c r="CY4" t="n">
         <v>878.63</v>
       </c>
-      <c r="AF4" t="n">
+      <c r="CZ4" t="n">
         <v>24.8</v>
       </c>
-      <c r="AG4" t="n">
+      <c r="DA4" t="n">
         <v>217.91</v>
       </c>
-      <c r="AH4" t="n">
+      <c r="DB4" t="n">
         <v>224.48</v>
       </c>
-      <c r="AI4" t="n">
+      <c r="DC4" t="n">
         <v>71.09999999999999</v>
       </c>
-      <c r="AJ4" t="n">
+      <c r="DD4" t="n">
         <v>0.8</v>
       </c>
-      <c r="AK4" t="n">
+      <c r="DE4" t="n">
         <v>99</v>
       </c>
-      <c r="AL4" t="n">
+      <c r="DF4" t="n">
         <v>198</v>
       </c>
     </row>
@@ -997,19 +2005,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0.88</v>
+        <v>13.13</v>
       </c>
       <c r="D5" t="n">
-        <v>1570.43</v>
+        <v>1396.23</v>
       </c>
       <c r="E5" t="n">
-        <v>67.05</v>
+        <v>67.2</v>
       </c>
       <c r="F5" t="n">
-        <v>1052.9</v>
+        <v>938.28</v>
       </c>
       <c r="G5" t="n">
-        <v>1215.79</v>
+        <v>943.67</v>
       </c>
       <c r="H5" t="n">
         <v>63.35</v>
@@ -1021,87 +2029,303 @@
         <v>150</v>
       </c>
       <c r="K5" t="n">
+        <v>140</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.96</v>
+      </c>
+      <c r="M5" t="n">
+        <v>1592.3</v>
+      </c>
+      <c r="N5" t="n">
+        <v>67.2</v>
+      </c>
+      <c r="O5" t="n">
+        <v>1070.04</v>
+      </c>
+      <c r="P5" t="n">
+        <v>1236.9</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>63.35</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="S5" t="n">
+        <v>150</v>
+      </c>
+      <c r="T5" t="n">
+        <v>140</v>
+      </c>
+      <c r="U5" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="V5" t="n">
+        <v>1570.43</v>
+      </c>
+      <c r="W5" t="n">
+        <v>67.05</v>
+      </c>
+      <c r="X5" t="n">
+        <v>1052.9</v>
+      </c>
+      <c r="Y5" t="n">
+        <v>1215.79</v>
+      </c>
+      <c r="Z5" t="n">
+        <v>63.35</v>
+      </c>
+      <c r="AA5" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AB5" t="n">
+        <v>150</v>
+      </c>
+      <c r="AC5" t="n">
         <v>138</v>
       </c>
-      <c r="L5" t="n">
+      <c r="AD5" t="n">
+        <v>27.36</v>
+      </c>
+      <c r="AE5" t="n">
+        <v>629.83</v>
+      </c>
+      <c r="AF5" t="n">
+        <v>81.06999999999999</v>
+      </c>
+      <c r="AG5" t="n">
+        <v>510.59</v>
+      </c>
+      <c r="AH5" t="n">
+        <v>529.24</v>
+      </c>
+      <c r="AI5" t="n">
+        <v>51.42</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>124</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>232</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>36.36</v>
+      </c>
+      <c r="AN5" t="n">
+        <v>552.24</v>
+      </c>
+      <c r="AO5" t="n">
+        <v>80.34999999999999</v>
+      </c>
+      <c r="AP5" t="n">
+        <v>443.75</v>
+      </c>
+      <c r="AQ5" t="n">
+        <v>452.41</v>
+      </c>
+      <c r="AR5" t="n">
+        <v>51.42</v>
+      </c>
+      <c r="AS5" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>125</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>234</v>
+      </c>
+      <c r="AV5" t="n">
         <v>5.78</v>
       </c>
-      <c r="M5" t="n">
+      <c r="AW5" t="n">
         <v>817.8099999999999</v>
       </c>
-      <c r="N5" t="n">
+      <c r="AX5" t="n">
         <v>80.34999999999999</v>
       </c>
-      <c r="O5" t="n">
+      <c r="AY5" t="n">
         <v>657.14</v>
       </c>
-      <c r="P5" t="n">
+      <c r="AZ5" t="n">
         <v>715.36</v>
       </c>
-      <c r="Q5" t="n">
+      <c r="BA5" t="n">
         <v>51.42</v>
       </c>
-      <c r="R5" t="n">
+      <c r="BB5" t="n">
         <v>1.7</v>
       </c>
-      <c r="S5" t="n">
+      <c r="BC5" t="n">
         <v>125</v>
       </c>
-      <c r="T5" t="n">
+      <c r="BD5" t="n">
         <v>234</v>
       </c>
-      <c r="U5" t="n">
+      <c r="BE5" t="n">
+        <v>5.04</v>
+      </c>
+      <c r="BF5" t="n">
+        <v>618.78</v>
+      </c>
+      <c r="BG5" t="n">
+        <v>60.56</v>
+      </c>
+      <c r="BH5" t="n">
+        <v>374.71</v>
+      </c>
+      <c r="BI5" t="n">
+        <v>418.06</v>
+      </c>
+      <c r="BJ5" t="n">
+        <v>93.34999999999999</v>
+      </c>
+      <c r="BK5" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="BL5" t="n">
+        <v>87</v>
+      </c>
+      <c r="BM5" t="n">
+        <v>154</v>
+      </c>
+      <c r="BN5" t="n">
+        <v>18.76</v>
+      </c>
+      <c r="BO5" t="n">
+        <v>527.28</v>
+      </c>
+      <c r="BP5" t="n">
+        <v>60.43</v>
+      </c>
+      <c r="BQ5" t="n">
+        <v>318.62</v>
+      </c>
+      <c r="BR5" t="n">
+        <v>324.82</v>
+      </c>
+      <c r="BS5" t="n">
+        <v>93.34999999999999</v>
+      </c>
+      <c r="BT5" t="n">
+        <v>2.05</v>
+      </c>
+      <c r="BU5" t="n">
+        <v>88</v>
+      </c>
+      <c r="BV5" t="n">
+        <v>156</v>
+      </c>
+      <c r="BW5" t="n">
         <v>0.82</v>
       </c>
-      <c r="V5" t="n">
+      <c r="BX5" t="n">
         <v>632.6799999999999</v>
       </c>
-      <c r="W5" t="n">
+      <c r="BY5" t="n">
         <v>61.16</v>
       </c>
-      <c r="X5" t="n">
+      <c r="BZ5" t="n">
         <v>386.95</v>
       </c>
-      <c r="Y5" t="n">
+      <c r="CA5" t="n">
         <v>458.96</v>
       </c>
-      <c r="Z5" t="n">
+      <c r="CB5" t="n">
         <v>93.34999999999999</v>
       </c>
-      <c r="AA5" t="n">
+      <c r="CC5" t="n">
         <v>2.05</v>
       </c>
-      <c r="AB5" t="n">
+      <c r="CD5" t="n">
         <v>89</v>
       </c>
-      <c r="AC5" t="n">
+      <c r="CE5" t="n">
         <v>152</v>
       </c>
-      <c r="AD5" t="n">
+      <c r="CF5" t="n">
+        <v>2.42</v>
+      </c>
+      <c r="CG5" t="n">
+        <v>1641.74</v>
+      </c>
+      <c r="CH5" t="n">
+        <v>35.23</v>
+      </c>
+      <c r="CI5" t="n">
+        <v>578.35</v>
+      </c>
+      <c r="CJ5" t="n">
+        <v>813.53</v>
+      </c>
+      <c r="CK5" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="CL5" t="n">
+        <v>0.64</v>
+      </c>
+      <c r="CM5" t="n">
+        <v>75</v>
+      </c>
+      <c r="CN5" t="n">
+        <v>148</v>
+      </c>
+      <c r="CO5" t="n">
+        <v>2.57</v>
+      </c>
+      <c r="CP5" t="n">
+        <v>1621.59</v>
+      </c>
+      <c r="CQ5" t="n">
+        <v>35.43</v>
+      </c>
+      <c r="CR5" t="n">
+        <v>574.5</v>
+      </c>
+      <c r="CS5" t="n">
+        <v>813.34</v>
+      </c>
+      <c r="CT5" t="n">
+        <v>67.5</v>
+      </c>
+      <c r="CU5" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="CV5" t="n">
+        <v>73</v>
+      </c>
+      <c r="CW5" t="n">
+        <v>144</v>
+      </c>
+      <c r="CX5" t="n">
         <v>43.72</v>
       </c>
-      <c r="AE5" t="n">
+      <c r="CY5" t="n">
         <v>931.12</v>
       </c>
-      <c r="AF5" t="n">
+      <c r="CZ5" t="n">
         <v>35.26</v>
       </c>
-      <c r="AG5" t="n">
+      <c r="DA5" t="n">
         <v>328.29</v>
       </c>
-      <c r="AH5" t="n">
+      <c r="DB5" t="n">
         <v>481.47</v>
       </c>
-      <c r="AI5" t="n">
+      <c r="DC5" t="n">
         <v>67.5</v>
       </c>
-      <c r="AJ5" t="n">
+      <c r="DD5" t="n">
         <v>0.63</v>
       </c>
-      <c r="AK5" t="n">
+      <c r="DE5" t="n">
         <v>74</v>
       </c>
-      <c r="AL5" t="n">
+      <c r="DF5" t="n">
         <v>146</v>
       </c>
     </row>
@@ -1117,19 +2341,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>56.38</v>
+        <v>37.03</v>
       </c>
       <c r="D6" t="n">
-        <v>640.63</v>
+        <v>923.9400000000001</v>
       </c>
       <c r="E6" t="n">
         <v>63.78</v>
       </c>
       <c r="F6" t="n">
-        <v>408.57</v>
+        <v>589.25</v>
       </c>
       <c r="G6" t="n">
-        <v>424.19</v>
+        <v>643.7</v>
       </c>
       <c r="H6" t="n">
         <v>35.76</v>
@@ -1144,84 +2368,300 @@
         <v>244</v>
       </c>
       <c r="L6" t="n">
+        <v>29.65</v>
+      </c>
+      <c r="M6" t="n">
+        <v>991.38</v>
+      </c>
+      <c r="N6" t="n">
+        <v>67.14</v>
+      </c>
+      <c r="O6" t="n">
+        <v>665.5700000000001</v>
+      </c>
+      <c r="P6" t="n">
+        <v>811.85</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>35.76</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="S6" t="n">
+        <v>146</v>
+      </c>
+      <c r="T6" t="n">
+        <v>246</v>
+      </c>
+      <c r="U6" t="n">
+        <v>56.38</v>
+      </c>
+      <c r="V6" t="n">
+        <v>640.63</v>
+      </c>
+      <c r="W6" t="n">
+        <v>63.78</v>
+      </c>
+      <c r="X6" t="n">
+        <v>408.57</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>424.19</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>35.76</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.66</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>146</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>244</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>23.94</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>230.01</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>164.87</v>
+      </c>
+      <c r="AG6" t="n">
+        <v>379.22</v>
+      </c>
+      <c r="AH6" t="n">
+        <v>394.79</v>
+      </c>
+      <c r="AI6" t="n">
+        <v>165.23</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>58</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>88</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>23.5</v>
+      </c>
+      <c r="AN6" t="n">
+        <v>234.15</v>
+      </c>
+      <c r="AO6" t="n">
+        <v>164.87</v>
+      </c>
+      <c r="AP6" t="n">
+        <v>386.04</v>
+      </c>
+      <c r="AQ6" t="n">
+        <v>397.57</v>
+      </c>
+      <c r="AR6" t="n">
+        <v>165.23</v>
+      </c>
+      <c r="AS6" t="n">
+        <v>1.75</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>58</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>88</v>
+      </c>
+      <c r="AV6" t="n">
         <v>24.57</v>
       </c>
-      <c r="M6" t="n">
+      <c r="AW6" t="n">
         <v>234.98</v>
       </c>
-      <c r="N6" t="n">
+      <c r="AX6" t="n">
         <v>164.87</v>
       </c>
-      <c r="O6" t="n">
+      <c r="AY6" t="n">
         <v>387.42</v>
       </c>
-      <c r="P6" t="n">
+      <c r="AZ6" t="n">
         <v>408.85</v>
       </c>
-      <c r="Q6" t="n">
+      <c r="BA6" t="n">
         <v>165.23</v>
       </c>
-      <c r="R6" t="n">
+      <c r="BB6" t="n">
         <v>1.75</v>
       </c>
-      <c r="S6" t="n">
+      <c r="BC6" t="n">
         <v>58</v>
       </c>
-      <c r="T6" t="n">
+      <c r="BD6" t="n">
         <v>88</v>
       </c>
-      <c r="U6" t="n">
+      <c r="BE6" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="BF6" t="n">
+        <v>613.71</v>
+      </c>
+      <c r="BG6" t="n">
+        <v>47.71</v>
+      </c>
+      <c r="BH6" t="n">
+        <v>292.79</v>
+      </c>
+      <c r="BI6" t="n">
+        <v>373.66</v>
+      </c>
+      <c r="BJ6" t="n">
+        <v>67.52</v>
+      </c>
+      <c r="BK6" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="BL6" t="n">
+        <v>133</v>
+      </c>
+      <c r="BM6" t="n">
+        <v>230</v>
+      </c>
+      <c r="BN6" t="n">
+        <v>0.43</v>
+      </c>
+      <c r="BO6" t="n">
+        <v>611.88</v>
+      </c>
+      <c r="BP6" t="n">
+        <v>47.85</v>
+      </c>
+      <c r="BQ6" t="n">
+        <v>292.76</v>
+      </c>
+      <c r="BR6" t="n">
+        <v>374.15</v>
+      </c>
+      <c r="BS6" t="n">
+        <v>67.52</v>
+      </c>
+      <c r="BT6" t="n">
+        <v>1.98</v>
+      </c>
+      <c r="BU6" t="n">
+        <v>132</v>
+      </c>
+      <c r="BV6" t="n">
+        <v>228</v>
+      </c>
+      <c r="BW6" t="n">
         <v>-15.81</v>
       </c>
-      <c r="V6" t="n">
+      <c r="BX6" t="n">
         <v>711.1799999999999</v>
       </c>
-      <c r="W6" t="n">
+      <c r="BY6" t="n">
         <v>47.85</v>
       </c>
-      <c r="X6" t="n">
+      <c r="BZ6" t="n">
         <v>340.27</v>
       </c>
-      <c r="Y6" t="n">
+      <c r="CA6" t="n">
         <v>363.37</v>
       </c>
-      <c r="Z6" t="n">
+      <c r="CB6" t="n">
         <v>67.52</v>
       </c>
-      <c r="AA6" t="n">
+      <c r="CC6" t="n">
         <v>1.98</v>
       </c>
-      <c r="AB6" t="n">
+      <c r="CD6" t="n">
         <v>132</v>
       </c>
-      <c r="AC6" t="n">
+      <c r="CE6" t="n">
         <v>228</v>
       </c>
-      <c r="AD6" t="n">
+      <c r="CF6" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="CG6" t="n">
+        <v>1738.42</v>
+      </c>
+      <c r="CH6" t="n">
+        <v>56.01</v>
+      </c>
+      <c r="CI6" t="n">
+        <v>973.67</v>
+      </c>
+      <c r="CJ6" t="n">
+        <v>1264.54</v>
+      </c>
+      <c r="CK6" t="n">
+        <v>62.97</v>
+      </c>
+      <c r="CL6" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="CM6" t="n">
+        <v>77</v>
+      </c>
+      <c r="CN6" t="n">
+        <v>148</v>
+      </c>
+      <c r="CO6" t="n">
+        <v>0.91</v>
+      </c>
+      <c r="CP6" t="n">
+        <v>1742.33</v>
+      </c>
+      <c r="CQ6" t="n">
+        <v>56.01</v>
+      </c>
+      <c r="CR6" t="n">
+        <v>975.86</v>
+      </c>
+      <c r="CS6" t="n">
+        <v>1267.54</v>
+      </c>
+      <c r="CT6" t="n">
+        <v>62.97</v>
+      </c>
+      <c r="CU6" t="n">
+        <v>0.79</v>
+      </c>
+      <c r="CV6" t="n">
+        <v>77</v>
+      </c>
+      <c r="CW6" t="n">
+        <v>148</v>
+      </c>
+      <c r="CX6" t="n">
         <v>1.54</v>
       </c>
-      <c r="AE6" t="n">
+      <c r="CY6" t="n">
         <v>1731</v>
       </c>
-      <c r="AF6" t="n">
+      <c r="CZ6" t="n">
         <v>56.01</v>
       </c>
-      <c r="AG6" t="n">
+      <c r="DA6" t="n">
         <v>969.52</v>
       </c>
-      <c r="AH6" t="n">
+      <c r="DB6" t="n">
         <v>1259.79</v>
       </c>
-      <c r="AI6" t="n">
+      <c r="DC6" t="n">
         <v>62.97</v>
       </c>
-      <c r="AJ6" t="n">
+      <c r="DD6" t="n">
         <v>0.79</v>
       </c>
-      <c r="AK6" t="n">
+      <c r="DE6" t="n">
         <v>77</v>
       </c>
-      <c r="AL6" t="n">
+      <c r="DF6" t="n">
         <v>148</v>
       </c>
     </row>

</xml_diff>